<commit_message>
Data Added for other subject
</commit_message>
<xml_diff>
--- a/DataSet/dataSetFormat.xlsx
+++ b/DataSet/dataSetFormat.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\3rd Sem\ITW\grade-calculator\DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9FF4CAC-5E72-4C38-B222-D49B48329622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BBDEE7-741B-4EB8-AEC4-8E80457DABC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AD45DF66-ED8C-4EA3-93EC-754FDC705C56}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="235">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -735,14 +735,17 @@
     <t>NAYAN Harsh</t>
   </si>
   <si>
-    <t>Total /*100</t>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>DSA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -762,16 +765,32 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Nunito"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF00FF"/>
+        <bgColor rgb="FFFF00FF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -794,24 +813,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{072CE35A-248A-4F39-A8EB-FF416F30DB40}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{7A1130D5-1772-4BD4-82CD-600DD1B101E9}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1123,10 +1161,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFBC3E4E-F312-492C-9082-865AFF87331C}">
-  <dimension ref="A1:D116"/>
+  <dimension ref="A1:E116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G113" sqref="G113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,7 +1175,7 @@
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1150,8 +1188,11 @@
       <c r="D1" s="3" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1164,8 +1205,11 @@
       <c r="D2" s="2">
         <v>67.777777777777771</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="5">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1178,8 +1222,11 @@
       <c r="D3" s="2">
         <v>81.111111111111114</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="5">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1192,8 +1239,11 @@
       <c r="D4" s="2">
         <v>77.777777777777771</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="5">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1206,8 +1256,11 @@
       <c r="D5" s="2">
         <v>71.111111111111114</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1220,8 +1273,11 @@
       <c r="D6" s="2">
         <v>67.777777777777771</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1234,8 +1290,11 @@
       <c r="D7" s="2">
         <v>58.888888888888886</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="5">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1248,8 +1307,11 @@
       <c r="D8" s="2">
         <v>31.111111111111111</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1262,8 +1324,11 @@
       <c r="D9" s="2">
         <v>62.222222222222221</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1276,8 +1341,11 @@
       <c r="D10" s="2">
         <v>64.444444444444443</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1290,8 +1358,11 @@
       <c r="D11" s="2">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1304,8 +1375,11 @@
       <c r="D12" s="2">
         <v>82.222222222222229</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1318,8 +1392,11 @@
       <c r="D13" s="2">
         <v>96.666666666666671</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1332,8 +1409,11 @@
       <c r="D14" s="2">
         <v>94.444444444444443</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1346,8 +1426,11 @@
       <c r="D15" s="2">
         <v>90</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1360,8 +1443,11 @@
       <c r="D16" s="2">
         <v>86.666666666666671</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1374,8 +1460,11 @@
       <c r="D17" s="2">
         <v>80</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1388,8 +1477,11 @@
       <c r="D18" s="2">
         <v>77.777777777777771</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="5">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1402,8 +1494,11 @@
       <c r="D19" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1416,8 +1511,11 @@
       <c r="D20" s="2">
         <v>93.333333333333329</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1430,8 +1528,11 @@
       <c r="D21" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1444,8 +1545,11 @@
       <c r="D22" s="2">
         <v>70</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1458,8 +1562,11 @@
       <c r="D23" s="2">
         <v>56.666666666666664</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="5">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1472,8 +1579,11 @@
       <c r="D24" s="2">
         <v>81.111111111111114</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1486,8 +1596,11 @@
       <c r="D25" s="2">
         <v>88.888888888888886</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1500,8 +1613,11 @@
       <c r="D26" s="2">
         <v>62.222222222222221</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1514,8 +1630,11 @@
       <c r="D27" s="2">
         <v>63.333333333333336</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1528,8 +1647,11 @@
       <c r="D28" s="2">
         <v>76.666666666666671</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1542,8 +1664,11 @@
       <c r="D29" s="2">
         <v>83.333333333333329</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1556,8 +1681,11 @@
       <c r="D30" s="2">
         <v>67.777777777777771</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1570,8 +1698,11 @@
       <c r="D31" s="2">
         <v>71.111111111111114</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="5">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1584,8 +1715,11 @@
       <c r="D32" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1598,8 +1732,11 @@
       <c r="D33" s="2">
         <v>77.777777777777771</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="5">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1612,8 +1749,11 @@
       <c r="D34" s="2">
         <v>81.111111111111114</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1626,8 +1766,11 @@
       <c r="D35" s="2">
         <v>94.444444444444443</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="5">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1640,8 +1783,11 @@
       <c r="D36" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="5">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1654,8 +1800,11 @@
       <c r="D37" s="2">
         <v>96.666666666666671</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="5">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -1668,8 +1817,11 @@
       <c r="D38" s="2">
         <v>86.666666666666671</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -1682,8 +1834,11 @@
       <c r="D39" s="2">
         <v>71.111111111111114</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -1696,8 +1851,11 @@
       <c r="D40" s="2">
         <v>83.333333333333329</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="5">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -1710,8 +1868,11 @@
       <c r="D41" s="2">
         <v>77.777777777777771</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" s="5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -1724,8 +1885,11 @@
       <c r="D42" s="2">
         <v>66.666666666666671</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" s="5">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -1738,8 +1902,11 @@
       <c r="D43" s="2">
         <v>62.222222222222221</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" s="5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -1752,8 +1919,11 @@
       <c r="D44" s="2">
         <v>63.333333333333336</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" s="5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -1766,8 +1936,11 @@
       <c r="D45" s="2">
         <v>77.777777777777771</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" s="5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -1780,8 +1953,11 @@
       <c r="D46" s="2">
         <v>87.777777777777771</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -1794,8 +1970,11 @@
       <c r="D47" s="2">
         <v>88.888888888888886</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" s="5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -1808,8 +1987,11 @@
       <c r="D48" s="2">
         <v>68.888888888888886</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" s="5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -1822,8 +2004,11 @@
       <c r="D49" s="2">
         <v>72.222222222222229</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" s="5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -1836,8 +2021,11 @@
       <c r="D50" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" s="5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -1850,8 +2038,11 @@
       <c r="D51" s="2">
         <v>67.777777777777771</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -1864,8 +2055,11 @@
       <c r="D52" s="2">
         <v>82.222222222222229</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" s="5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -1878,8 +2072,11 @@
       <c r="D53" s="2">
         <v>63.333333333333336</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" s="5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -1892,8 +2089,11 @@
       <c r="D54" s="2">
         <v>52.222222222222221</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" s="5">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -1906,8 +2106,11 @@
       <c r="D55" s="2">
         <v>76.666666666666671</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55" s="5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -1920,8 +2123,11 @@
       <c r="D56" s="2">
         <v>61.111111111111114</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" s="5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -1934,8 +2140,11 @@
       <c r="D57" s="2">
         <v>75.555555555555557</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" s="5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -1948,8 +2157,11 @@
       <c r="D58" s="2">
         <v>83.333333333333329</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" s="5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -1962,8 +2174,11 @@
       <c r="D59" s="2">
         <v>74.444444444444443</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" s="5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -1976,8 +2191,11 @@
       <c r="D60" s="2">
         <v>81.111111111111114</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" s="5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -1990,8 +2208,11 @@
       <c r="D61" s="2">
         <v>87.777777777777771</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" s="5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -2004,8 +2225,11 @@
       <c r="D62" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" s="5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -2018,8 +2242,11 @@
       <c r="D63" s="2">
         <v>83.333333333333329</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63" s="5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -2032,8 +2259,11 @@
       <c r="D64" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" s="5">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -2046,8 +2276,11 @@
       <c r="D65" s="2">
         <v>60</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" s="5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -2060,8 +2293,11 @@
       <c r="D66" s="2">
         <v>91.111111111111114</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" s="5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -2074,8 +2310,11 @@
       <c r="D67" s="2">
         <v>81.111111111111114</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67" s="5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -2088,8 +2327,11 @@
       <c r="D68" s="2">
         <v>61.111111111111114</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" s="5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -2102,8 +2344,11 @@
       <c r="D69" s="2">
         <v>67.777777777777771</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69" s="5">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -2116,8 +2361,11 @@
       <c r="D70" s="2">
         <v>74.444444444444443</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70" s="5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -2130,8 +2378,11 @@
       <c r="D71" s="2">
         <v>74.444444444444443</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71" s="5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -2144,8 +2395,11 @@
       <c r="D72" s="2">
         <v>60</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72" s="5">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -2158,8 +2412,11 @@
       <c r="D73" s="2">
         <v>81.111111111111114</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -2172,8 +2429,11 @@
       <c r="D74" s="2">
         <v>57.777777777777779</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -2186,8 +2446,11 @@
       <c r="D75" s="2">
         <v>62.222222222222221</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75" s="5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -2200,8 +2463,11 @@
       <c r="D76" s="2">
         <v>63.333333333333336</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76" s="5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -2214,8 +2480,11 @@
       <c r="D77" s="2">
         <v>55.555555555555557</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77" s="5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -2228,8 +2497,11 @@
       <c r="D78" s="2">
         <v>55.555555555555557</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78" s="5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -2242,8 +2514,11 @@
       <c r="D79" s="2">
         <v>84.444444444444443</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79" s="5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -2256,8 +2531,11 @@
       <c r="D80" s="2">
         <v>68.888888888888886</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80" s="5">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -2270,8 +2548,11 @@
       <c r="D81" s="2">
         <v>43.333333333333336</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81" s="5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -2284,8 +2565,11 @@
       <c r="D82" s="2">
         <v>81.111111111111114</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82" s="5">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -2298,8 +2582,11 @@
       <c r="D83" s="2">
         <v>58.888888888888886</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83" s="5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>83</v>
       </c>
@@ -2312,8 +2599,11 @@
       <c r="D84" s="2">
         <v>67.777777777777771</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84" s="5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -2326,8 +2616,11 @@
       <c r="D85" s="2">
         <v>72.222222222222229</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85" s="5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -2340,8 +2633,11 @@
       <c r="D86" s="2">
         <v>67.777777777777771</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86" s="5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -2354,8 +2650,11 @@
       <c r="D87" s="2">
         <v>76.666666666666671</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -2368,8 +2667,11 @@
       <c r="D88" s="2">
         <v>84.444444444444443</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88" s="5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -2382,8 +2684,11 @@
       <c r="D89" s="2">
         <v>68.888888888888886</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89" s="5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -2396,8 +2701,11 @@
       <c r="D90" s="2">
         <v>55.555555555555557</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90" s="5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -2410,8 +2718,11 @@
       <c r="D91" s="2">
         <v>73.333333333333329</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E91" s="5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -2424,8 +2735,11 @@
       <c r="D92" s="2">
         <v>77.777777777777771</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92" s="5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -2438,8 +2752,11 @@
       <c r="D93" s="2">
         <v>93.333333333333329</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93" s="5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>93</v>
       </c>
@@ -2452,8 +2769,11 @@
       <c r="D94" s="2">
         <v>50</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94" s="5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -2466,8 +2786,11 @@
       <c r="D95" s="2">
         <v>81.111111111111114</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95" s="6">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -2480,8 +2803,11 @@
       <c r="D96" s="2">
         <v>64.444444444444443</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96" s="5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -2494,8 +2820,11 @@
       <c r="D97" s="2">
         <v>85.555555555555557</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97" s="5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -2508,8 +2837,11 @@
       <c r="D98" s="2">
         <v>54.444444444444443</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -2522,8 +2854,11 @@
       <c r="D99" s="2">
         <v>76.666666666666671</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -2536,8 +2871,11 @@
       <c r="D100" s="2">
         <v>80</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -2550,8 +2888,11 @@
       <c r="D101" s="2">
         <v>82.222222222222229</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
         <v>101</v>
       </c>
@@ -2564,8 +2905,11 @@
       <c r="D102" s="2">
         <v>65.555555555555557</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E102" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -2578,8 +2922,11 @@
       <c r="D103" s="2">
         <v>84.444444444444443</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E103" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
         <v>103</v>
       </c>
@@ -2592,8 +2939,11 @@
       <c r="D104" s="2">
         <v>45.555555555555557</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E104" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A105" s="2">
         <v>104</v>
       </c>
@@ -2606,8 +2956,11 @@
       <c r="D105" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E105" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A106" s="2">
         <v>105</v>
       </c>
@@ -2620,8 +2973,11 @@
       <c r="D106" s="2">
         <v>45.555555555555557</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E106" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
         <v>106</v>
       </c>
@@ -2634,8 +2990,11 @@
       <c r="D107" s="2">
         <v>56.666666666666664</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E107" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A108" s="2">
         <v>107</v>
       </c>
@@ -2648,8 +3007,11 @@
       <c r="D108" s="2">
         <v>72.222222222222229</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E108" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A109" s="2">
         <v>108</v>
       </c>
@@ -2662,8 +3024,11 @@
       <c r="D109" s="2">
         <v>42.222222222222221</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E109" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A110" s="2">
         <v>109</v>
       </c>
@@ -2676,8 +3041,11 @@
       <c r="D110" s="2">
         <v>16.666666666666668</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E110" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A111" s="2">
         <v>110</v>
       </c>
@@ -2690,8 +3058,11 @@
       <c r="D111" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E111" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A112" s="2">
         <v>111</v>
       </c>
@@ -2704,8 +3075,11 @@
       <c r="D112" s="2">
         <v>55.555555555555557</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E112" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A113" s="2">
         <v>112</v>
       </c>
@@ -2718,8 +3092,11 @@
       <c r="D113" s="2">
         <v>70</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E113" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A114" s="2">
         <v>113</v>
       </c>
@@ -2732,8 +3109,11 @@
       <c r="D114" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E114" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A115" s="2">
         <v>114</v>
       </c>
@@ -2746,8 +3126,11 @@
       <c r="D115" s="2">
         <v>74.444444444444443</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E115" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A116" s="2">
         <v>115</v>
       </c>
@@ -2758,6 +3141,9 @@
         <v>232</v>
       </c>
       <c r="D116" s="2">
+        <v>0</v>
+      </c>
+      <c r="E116" s="7">
         <v>0</v>
       </c>
     </row>

</xml_diff>